<commit_message>
HAJ-944 , HAJ-942 , HAJ-937, HAJ-951  emergency data issues
</commit_message>
<xml_diff>
--- a/shj-admin-portal-web/src/main/resources/templates/excel/7/applicant-emergency-data.xlsx
+++ b/shj-admin-portal-web/src/main/resources/templates/excel/7/applicant-emergency-data.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aabdelmoula\Downloads\Valid_Haj_input_07\Valid_Haj_input_07\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SmartHajj\smart-hajj\shj-admin-portal-web\src\main\resources\templates\excel\7\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
   </bookViews>
   <sheets>
-    <sheet name="Applicant Data" sheetId="1" r:id="rId1"/>
+    <sheet name="applicant emergency data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>PassportNo
 	رقم الجواز</t>
@@ -131,86 +131,8 @@
 YYYYMMDD</t>
   </si>
   <si>
-    <t>14051016</t>
-  </si>
-  <si>
-    <t>18/02/1987</t>
-  </si>
-  <si>
-    <t>Khaled_Abdelaziz_Abdelaziz_Elsayed</t>
-  </si>
-  <si>
-    <t>خالد عبدالعزيز عبدالعزيز السيد</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>ae</t>
-  </si>
-  <si>
-    <t>1236521452365461</t>
-  </si>
-  <si>
-    <t>/9j/4AAQSkZJRgABAAEASABIAAD//gAfTEVBRCBUZWNobm9sb2dpZXMgSW5jLiBWMS4wMQD/2wCEAAUFBQgFCAwHBwwMCQkJDA0MDAwMDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NDQ0BBQgICgcKDAcHDA0MCgwNDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NDf/EAaIAAAEFAQEBAQEBAAAAAAAAAAABAgMEBQYHCAkKCwEAAwEBAQEBAQEBAQAAAAAAAAECAwQFBgcICQoLEAACAQMDAgQDBQUEBAAAAX0BAgMABBEFEiExQQYTUWEHInEUMoGRoQgjQrHBFVLR8CQzYnKCCQoWFxgZGiUmJygpKjQ1Njc4OTpDREVGR0hJSlNUVVZXWFlaY2RlZmdoaWpzdHV2d3h5eoOEhYaHiImKkpOUlZaXmJmaoqOkpaanqKmqsrO0tba3uLm6wsPExcbHyMnK0tPU1dbX2Nna4eLj5OXm5+jp6vHy8/T19vf4+foRAAIBAgQEAwQHBQQEAAECdwABAgMRBAUhMQYSQVEHYXETIjKBCBRCkaGxwQkjM1LwFWJy0QoWJDThJfEXGBkaJicoKSo1Njc4OTpDREVGR0hJSlNUVVZXWFlaY2RlZmdoaWpzdHV2d3h5eoKDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uLj5OXm5+jp6vLz9PX29/j5+v/AABEIAGwATwMBEQACEQEDEQH/2gAMAwEAAhEDEQA/APbdWkvGMS2JljPmIHKpG8bLI2xxISwki8pMypKuFD7Qd33DlBR+15+q9O/axtbRtWuujdv69NzobcMIQrgqVyo3NvYhSVVmYdWYAM3+0TnmpkknaLuu9rev3PQzT7q3kQOApAOBuzgHvgZOB345OO3PSsjQggtEgUxoMKSxx0xu64xjH4fzpFbGfa2Is52UI3zl2WRpC55VFIOT2CKACCQAPmJyTTk2uXp2t6/5sNG+a1n5afhsRXs0kMyQxKG8zduJVyVABbKgAK4wrKw3qQzJ1BwVGClu7eui/wCB/wAOU7pX6eX+W5LdrACpkCKFyQX28EqcgZ/i27s45xu7ZrK3RDRx974A0q8mF9DELacAsHi+VDuH3mj+4Tg8EBT71lKF1YtS5Xc5XxdoOoGBYbJPOjXAYIQH2oBtG0kE5OWbbnkDiohHkevyKk77Hj8tu9s2yZWiYdQ6lT+RANbGZ9ofZkuBskztPoSD+nX6HI9q69jnLNvbNax7GJb5iRk/w9h6D8APXryRknKm1Sz1Jp5ZFR5hHjaj8kFgxIdmRHePy4i0QBZFO7GQBfMuXltffrtf03V9bPqW+nK2rbrR/c99fwOlmlW1Xe4YjIB2jcQD/EQOdo/iIzj0rJR5nZbj2LQXeoP9QcHuMjjg8HFJq2jC5m39n9oTZllI5Ug4wexI6H8RU7FGVf6b9piQMDKYmR9uVwxjZWyS4JByvDKQ2CwzyacXyu6/q5XRr/h0StIyWu9VbIXhTuc56DdjLkZ5bGW25wMioer6fLRAl0X4nNafdz3sIluU8p2AbaOg3D7oz8+V6kuqN823b8pJiaUfhd/66/8AAuWuqatb0/QzruW2upTayeXM6/ejYK5TgMC4IOzIIKlsbugyazs1qWdnYancXFy6bVMETIFMQcllmGU83zFUxNCqlpAud28DC4Ab1eRJXuk7PR6bdu9+hxSvFpNP9PvOtk5ArERTkjjuBtOGCP2Odrr29mB6jqO9LYomFus2NwBKnIJGcH29P85zSWmw722LYjwMen4U2JGMqsszh33ZJwp6hRjaBjC8ZYk43HIBPyinLlsrJ3/Dz8+34lemw1bhTKYQCNvU9QSRkYxn0bO7bjA4O4VPI7c3Qe2hBfEIhLYVe5PA545PbPSsWUjkYLCKyd2hG0PjK84GPTJOM9SKyNNjnb/T3iuDcRRpMH2gh2dmG3zCMZOAuZG4B7+gAFqTSsnZf1/kNpOzaWh6ne2skrCSGRlYEfLkbcDrjpg/XNdhxl2eH7ZC0LbSrAhgy71Ze6lQQefY59KFo7jTSev+RkQ3MOk2jBmcCBEB8zj7q4LAHnLnLHJYnuac5J62StfbzEk72Tbv3OW0b4jWt3ftZEFR8ux/mwSSQQwKgDkEqVZsjnjisYyhJfEk9dH19DaVOUeh6u0kccbTSMscaKXZ2IVVVRlmZjgKoHJJIAFXYyOFsvHnh3WL0WFlewy3bZVEw6eZ6iNnRVkOOQFJJH3c1PoXZx3VjpHgPmbwxA7r2NIDifF9sXMM4DyCAudse0EBkYFsk8gEq+3Y/wA0asNpHJzcvRP1K3VtU+6ZXuJnS2MsKlpNmUUgsckcbwpDEf3tpz6VhbXXT8DVdvzM61mluIRJOFVzgkKysBuUNtG3+4SUy3zNt3EDOA5JJ+67r0t/XclN9Vb8fyO60q7kvohJIpQsFkX5SoCSjeiA5O9o1IWRxhS/KjFd8ocnVPfZ320/HocSlfZNW7qxsrKkWFLAMRkL1YgkLkKPmIyQCQMDvUWLPPPiXO0NqsS8bz8x6ZA7e9cdd2jY6qC96/Y8b0TSP7Y1K3jQsrK4YkE4CqckY6c9M1xUk3JJHZUajFtnr/xe1GS30OOxiGEvZ1ilOcHZEvnbOnIlZArf7II5zXpTfKtDjoQU52b21t3PCdCzdxqXh3Ss7+XJwRHIhBjkz95cMflxyCO3SvNtaV4u23ke9bmg1KN/i7O1l+B9cQSl48swZl+8cEc4G7OffJ44AIAAxXqyt9nQ+aRyo1MajJIioypGzIHyGDFdpJDLlQpV0IBYPu3qUGwkzKNlfT9fu36ehez5Xe/o/wDhipLJFGfLkZRvwApIy247QNvUgkhemMnBrOxRV+yQ2oIhUJvbcQOB0xwOw9qljOt06ylsnYNK00ZAC7zyD057dOAa7jkNO9CWkL3TruESMxyQNqhSDg8NyCeN3JNUpOGq0/q491y2/O58x+KPF8+vktgRQgYjjBwVXoCWIPIHPTHbmvGqTdSXlf8Ar7z1acFTXmecaJ40vPDtz9ohCTOuQd5OHPrldvYAfKAOMgcmu2EFB80dPI5ZvmXK++5p+IfiDq3j1UsZlggEDiWJIlbc8gDAksxZiAh2lRtHzZOTirm9NduoqStK0d+h13gO8stH1OGDVpY7MRKG27xIGmdxsErjCwL/ABnccnaA23I3csIpvmfTbSx31qsox9nFWutdbu3/AAfvPqQFWXemCH+YMpBDZ7gjgj3FdR5Rz09iouPtKs+SCGXcSpz0IGcDGOg4qSjldZ04yzJdxoJnjV12sxXCuArbNqhuQDkbwpyx2knIak4fCNpNWa/NP8C45diSq7zgYUELkn73J4GBzz16Vnb5F/gdxb7mClgVJAO04yCRnBxxkHg4OM9DXbscZ5p458c2/wBifT7fcJZWMTb1aNlKcyL5bhX+4VYPjYVddrEkgY17whtvt6P+rHRRSc91prb8T5b1rUST5aHk8fh/9euSlDqzqqS6I49ZcsVH8P8APrXbY5bnZeGLY3EcssZKSpLEEdeGUsQMqe3BOex7g1jPt0C9mmtGtg1i0ihv2WIDd5Q8w9cs7ZyxPViBk+vU0obWWy2K1b5nuz2f4TSXN7Z6jpiyyKsYgkiVWbKE7w3lESR+WSwQ8NtJHzKwJB2Xuu9ri06/1+DPbbdgLf5UdAhYBDtDDBOFUDauB91eg9T3qXq7pWJStpf5nL2F9PdNILkRqyswCoQCArlQShLMC64c5YheAOppSSWz17f8EeqbXTvfc1bJ4xcpC5w0u/YuD821ckZxtBA5wSCQCQDg1KTew3odJFGlvb+XMdyJGQ5YnlcHcSevIzmuvY59tj5B8V6m13fTXEJVIHkfagGMKcDOSWJLYBJJ9AMDAHnSl7WV3029D0VeC1er3PNXk8x2kPRAT+PauuK5VY5WzBtspnd13HP1q2Sj0LwderaW11K52iF0kJ6dFbaB7kkY9T0rGQMtaXBJLBeazPayXFuqOXcFglu8mBC8jL/cGWVCQCSAcjg1FcqsVc9O+Bd0/wBqujsZvOgjLYH3R5vHHr8yj0wGJPAB05b9Urd3Yhu1t/kfQmpXEVjH5k7rGpYKCxxlj91R6s2MKByTwOazt0QznGgi8zz41Cs64yBgkE55A75655B4NQ1YpGtaWGQbmPEcygKj7QSMnn/x3I/E+tNXWwN9OhynxM8QtoWjssIDT3bCJVJKnYceYwIVuQCODtGCTuGK2npFq9r6EU027pXtqfKN/cMUJb+EEZGOccZ44GeuB06ZNccIpPQ6ZO5z5fyIN59yfw5H64rrOcx7ZcgDv/U0xmxZxOXa3ORG213A6MEztB/Fv51LWwbHrQ1qBvBWp6EiyRS7lvZp8r5bqs0EUUG0fMMkrkngYJ6HFUiWdP8AAqzW7kvHfK4jhKEEggeYcDj1C8g+tJg9D3/XLVbuPYcKwIZSQSoIZWGVDKGG5VOGyOOlK7jtoC2a6PcxbRXRFjk2b1B+6ML1OMAdB6496h6u73GlZWWiKuo6tL4a0+eeZnkkVlKbl+TEkihUQkAkKvmEDGccEsFU1Tatoref/ADrpt2OF8eo2v6vb6Qf9Sihn545+ZyceijFRUvKaguhcLRg5Hz94hEUTzC2GyIyFYx/sg4H6DNC+LToVsjlNTwsccffr+H/AOv+VbGRWiXBwB079APc0DN7TdzxGfJ+bJAA/hUkDHf1P40CO3gXb4e1onndFYrnuC14nHvnH6U0J9D1r4HWrQ211Nt+UmKPdnuisxUD/gYJNITPTL+e4ivh5shEDBRHGFLLuJYNlgqYLLtwHaUK25l28Ue7a1nf+v66C7cr9br8nf8AQS4ulsh5xRpTuACJjcckDjOBkZzjOT0GTUpXdi/TocX8VtSLQ2dhjaW3TyL6bf3aD6ElyM4JGCQDwJkrafkKOuo3xBo76feXesv5rbocRKmGEZJKli/ljYJEABUM7YZ1JUYz02ULytdtPV3009enQybvywTdrq6svu/z2PABFbyMq3Qyu4Nz7cnp6jivLbktYbnqwUG7VNjI8d21rBfRR2SiOMRfMoJI3B2G7knhwARz09K2ouUo3nvcjEQjTklT0Vr736s5a4Iih2LxnG4/0rpOM6mwjEVvDjsg/UZ/rTFsdZLYyy+HZfJRnkv9RtoVCjqlrFJO/fu7xjv0pNqKu3YqMXN+6r2WyPf/AIZ2raToQM6mJnllkYMNpwMIv3sdQvGcA560b7ENO9ra9up2NrqUeq25mRHReq7xgkc4PdQchhhWbjDZwwpyi47/AJkJ6tdtHo1+Y6yWKU+VIQS/GzOCep6Ag4wD7HBqLFHgPja5W61eZIv9Va4t4xnPEYw3Pu5es2aI9j8R6jDd6RdNbuHVYzhlIKsGBw6MpIZCQwBB5KtxjBPbUTjBtq17/hv+Zyws526p6+R8iX9wsREZBJIyODjA6846gc46nj1rzYq56EnY5q7UtchT2x+ozj9f1rpitDJnQXWghdDutYcFY4ZYLWI8/PPKdz+xEcKsT/tOnoa1tpcyb1sinply8yJHtHACqP4jgYHtk8Uij6RuvAxEWnaVbXaQPalZrqM5L75WWR5FwMAOyJCgOBhAgJLms50nNabK/wDwX8kdFGtGjdtO7atqunT7z2GKBLOAIDhI15LEDjqWY9B3JPQVSSilFbI5pSc5Ob3buZn2RLPd5ZfEmPlZiwHrjJ4z6UhEclqunb9Y+T9xCxcuCW2p84CdAPnVcA55ORjnNJuKstF1BpO2m2x8zszTMZHPzSMWbnqzEsf1NYGp7zr1n/Yui3AeTfCkQSOMDaFOcD3Y88seTyTjNddVvlbkznpr3lZJa300PlhrIahcJCMqXPzMMDCgZYk9cKoJ644rgh2Oybsjl4pluLh5V+7lmHrjPH44wK7EYbHtvxQij8L+E9L0BFLTX0i3cxJ6NGm98Dr80k4XPYIRWktEkYx1bZx/wq0f+1tbt1kAZIj5zAfdCRfPgD0LBAT3JqEavRH17Ppxe4FzEQjnAfcu7I3bjgsTs5JICgDPJ7Yq72T0Ietr2020Wg/WNMN8sZUBmgkEiqTtUsvqwUt04wCoIODxST5dg6Nd/Npr7iAI5RF27XVB8pYkA4wAWOT9ScnvzUPV3Y1poc14jN8+hS2vzTXM0iRt8nljYGLtsB2hgUVAdqqCxYgfNU1JRitE/wCv68y4ptva3Tp/meDTRNbt5cqtGw6hgQf1/pWCknszVpx3PYfiTfSHQoiMD7Q8e8DPdd2BzwM+ueK68T7qcV3sc1DV38j560BD5Gr3LEtLa2E/lk443skZPAHIR2Axjqc5rOmkle3Q0m3dLzOT0O3SScIw4eSFD/uswB/Q1otCWeuftCNt1yzg/wCWcFgNg9N08gP6Io/CrnuZ09jsPgFpsJ0+61Mgm5klEG84+WNVD7UGPlBYgt67V9KlFS7HsPhq4luVcTuZWVmG5sAnbNNEDhQqj5Y1yFVVLZbGWJPTUgoxjJdb/lF/qc8JuUpxdrRdl+P+RYt9Tln1S4sCFEVsItuAdzebHvO4kn7pHy7QowTu3HBGPKrX9fwaX6m70t53L8aDzmPoayGcX481GazubaOMgJ5TMVIyCS+P5DjFcNdtNJdmdlFJp+pkeVHfRKZ0R8jOCMj8M5P61ynRtoj/2Q==</t>
-  </si>
-  <si>
-    <t>/9j/4QaVRXhpZgAATU0AKgAAAAgABwESAAMAAAABAAEAAAEaAAUAAAABAAAAYgEbAAUAAAABAAAAagEoAAMAAAABAAIAAAExAAIAAAAfAAAAcgEyAAIAAAAUAAAAkYdpAAQAAAABAAAAqAAAANQAbd0AAAAnEABt3QAAACcQQWRvYmUgUGhvdG9zaG9wIDIxLjAgKFdpbmRvd3MpADIwMjE6MDU6MDUgMTQ6MTY6MDMAAAAAAAOgAQADAAAAAQABAACgAgAEAAAAAQAAAtagAwAEAAAAAQAAAtYAAAAAAAAABgEDAAMAAAABAAYAAAEaAAUAAAABAAABIgEbAAUAAAABAAABKgEoAAMAAAABAAIAAAIBAAQAAAABAAABMgICAAQAAAABAAAFWwAAAAAAAABIAAAAAQAAAEgAAAAB/9j/7QAMQWRvYmVfQ00AAf/uAA5BZG9iZQBk</t>
-  </si>
-  <si>
-    <t>widowed</t>
-  </si>
-  <si>
-    <t>NON</t>
-  </si>
-  <si>
-    <t>ar,en,fr</t>
-  </si>
-  <si>
-    <t>aelsayed@elm.sa</t>
-  </si>
-  <si>
-    <t>0551367745</t>
-  </si>
-  <si>
-    <t>00204825566336644</t>
-  </si>
-  <si>
-    <t>545454</t>
-  </si>
-  <si>
-    <t>eg</t>
-  </si>
-  <si>
-    <t>1236521452365462</t>
-  </si>
-  <si>
-    <t>married</t>
-  </si>
-  <si>
     <t>PackageCode
 باقة الشركة</t>
-  </si>
-  <si>
-    <t>PKG1442</t>
-  </si>
-  <si>
-    <t>1010101054</t>
-  </si>
-  <si>
-    <t>1010101055</t>
-  </si>
-  <si>
-    <t>A22254</t>
-  </si>
-  <si>
-    <t>A22255</t>
-  </si>
-  <si>
-    <t>Ahmed Elsayed Fouad Elsayed</t>
-  </si>
-  <si>
-    <t>اخمد السيد فؤاد السيد</t>
   </si>
   <si>
     <t>GroupReferenceNumber
@@ -239,33 +161,6 @@
   <si>
     <t>SeatNumber
 رقم المقعد</t>
-  </si>
-  <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>1234567891225678912345678912345678912345678912365</t>
-  </si>
-  <si>
-    <t>3123456789</t>
-  </si>
-  <si>
-    <t>6566</t>
-  </si>
-  <si>
-    <t>963216</t>
-  </si>
-  <si>
-    <t>963215</t>
-  </si>
-  <si>
-    <t>3123456790</t>
-  </si>
-  <si>
-    <t>5616</t>
-  </si>
-  <si>
-    <t>124</t>
   </si>
 </sst>
 </file>
@@ -524,7 +419,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
+    <cellStyle name="20 % - Accent1" xfId="1" builtinId="30"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="38">
@@ -1594,7 +1489,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B3:AH999" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33" headerRowCellStyle="20% - Accent1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B3:AH999" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
   <autoFilter ref="B3:AH999"/>
   <tableColumns count="33">
     <tableColumn id="2" name="ID Number _x000a__x0009_رقم الهوية الوطنية / الإقامة" dataDxfId="32"/>
@@ -1636,7 +1531,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1900,11 +1795,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:AH999"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AD8" sqref="AD8"/>
+    <sheetView tabSelected="1" topLeftCell="A940" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I3" sqref="B3:AH999"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.1796875" style="2"/>
     <col min="2" max="2" width="25.54296875" style="2" customWidth="1"/>
@@ -2008,231 +1903,99 @@
         <v>14</v>
       </c>
       <c r="AA3" s="7" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="AB3" s="13" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="AC3" s="14" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="AD3" s="14" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="AE3" s="14" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="AF3" s="14" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="AG3" s="14" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="AH3" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="2:34" x14ac:dyDescent="0.35">
-      <c r="B4" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="L4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="M4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="V4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="X4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z4" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA4" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB4" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC4" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="AD4" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE4" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="AF4" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="AG4" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="AH4" s="19" t="s">
-        <v>59</v>
-      </c>
+    </row>
+    <row r="4" spans="2:34" x14ac:dyDescent="0.35">
+      <c r="B4" s="9"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="10"/>
+      <c r="AA4" s="12"/>
+      <c r="AB4" s="12"/>
+      <c r="AC4" s="15"/>
+      <c r="AD4" s="15"/>
+      <c r="AE4" s="15"/>
+      <c r="AF4" s="15"/>
+      <c r="AG4" s="16"/>
+      <c r="AH4" s="19"/>
     </row>
     <row r="5" spans="2:34" x14ac:dyDescent="0.35">
-      <c r="B5" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="R5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="S5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="T5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="U5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="V5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="W5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="X5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z5" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA5" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB5" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC5" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD5" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="AE5" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="AF5" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="AG5" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="AH5" s="3" t="s">
-        <v>67</v>
-      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="10"/>
+      <c r="AA5" s="12"/>
+      <c r="AB5" s="12"/>
+      <c r="AC5" s="17"/>
+      <c r="AD5" s="17"/>
+      <c r="AE5" s="17"/>
+      <c r="AF5" s="15"/>
+      <c r="AG5" s="18"/>
+      <c r="AH5" s="3"/>
     </row>
     <row r="6" spans="2:34" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="9"/>

</xml_diff>